<commit_message>
update xlsx, driver js
</commit_message>
<xml_diff>
--- a/db/data_base.xlsx
+++ b/db/data_base.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
   <si>
     <t>animals_name</t>
   </si>
@@ -126,7 +126,7 @@
     <t>f686c2a9-233d-4b90-978f-6fa28973d43b</t>
   </si>
   <si>
-    <t>completed</t>
+    <t>1 pending</t>
   </si>
   <si>
     <t>de47e3d8-338b-4b4c-bc13-3ffd6c8106f3</t>
@@ -150,6 +150,9 @@
     <t>52afb9e4-a647-4417-90d2-8351ee950313</t>
   </si>
   <si>
+    <t>2 driver accepts</t>
+  </si>
+  <si>
     <t>641a1732-f6e1-4385-94e9-8e24f2c17429</t>
   </si>
   <si>
@@ -174,7 +177,7 @@
     <t>db6abe0e-6b32-4436-b7de-db1c7fa953c3</t>
   </si>
   <si>
-    <t>cancelled</t>
+    <t>3 driver delivering</t>
   </si>
   <si>
     <t>f25d018e-6f07-46de-a34d-4d8b9456883f</t>
@@ -198,6 +201,9 @@
     <t>917542c7-7c2e-4a2d-a256-199b17e7261b</t>
   </si>
   <si>
+    <t>4 receiver received</t>
+  </si>
+  <si>
     <t>b57ccb86-8291-415f-8e8e-50d8f18eecfd</t>
   </si>
   <si>
@@ -214,6 +220,9 @@
   </si>
   <si>
     <t>bf54a164-46ee-45ec-a776-6e690994b191</t>
+  </si>
+  <si>
+    <t>5 cancelled</t>
   </si>
   <si>
     <t>97689a33-ee84-44c6-a2b1-d40e5f0fc05f</t>
@@ -313,11 +322,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="hh:mm"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode=": yymd"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode=": yymd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -340,12 +348,17 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFffffff"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -357,55 +370,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FFff0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFff0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFff0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFff0000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="167" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -414,20 +411,38 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,10 +469,10 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4285F4"/>
@@ -731,132 +746,198 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="17.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="18">
+        <v>80</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="9">
         <v>51170071</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="6"/>
+        <v>96</v>
+      </c>
+      <c r="I2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="18">
+      <c r="F3" s="9">
         <v>93493702</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="18">
+        <v>90</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="9">
         <v>51906988</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="13.550000000000002">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="13.550000000000002">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="13.550000000000002">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="13.550000000000002">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="13.550000000000002">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="13.550000000000002">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -868,125 +949,185 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="19" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="18">
+        <v>80</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="9">
         <v>51170071</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="9">
+        <v>93493702</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="18">
-        <v>93493702</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="18">
+        <v>90</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="9">
         <v>51906988</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="13.550000000000002">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="13.550000000000002">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="13.550000000000002">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="13.550000000000002">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="13.550000000000002">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="13.550000000000002">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1004,25 +1145,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="38.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="37.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="15" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="15" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="38.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="14" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="14" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1047,10 +1188,10 @@
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -1072,33 +1213,33 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
+      <c r="A2" s="8"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="J2" s="9">
-        <v>12345678</v>
-      </c>
-      <c r="K2" s="3">
+        <v>51170071</v>
+      </c>
+      <c r="K2" s="4">
         <v>20</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="4">
         <v>10</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -1114,243 +1255,243 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J3" s="9">
-        <v>23456789</v>
-      </c>
-      <c r="K3" s="3">
+        <v>93493702</v>
+      </c>
+      <c r="K3" s="4">
         <v>32</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="4">
         <v>10</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
+      <c r="A4" s="8"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="9">
+        <v>51906988</v>
+      </c>
+      <c r="K4" s="4">
         <v>45</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="L4" s="4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21.75">
+      <c r="A5" s="8"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="9">
-        <v>34567890</v>
-      </c>
-      <c r="K4" s="3">
-        <v>45</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="9">
+        <v>51170071</v>
+      </c>
+      <c r="K5" s="4">
         <v>10</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="9">
-        <v>12345678</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="L5" s="4">
         <v>10</v>
       </c>
-      <c r="L5" s="3">
-        <v>10</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21.75">
+      <c r="A6" s="8"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="J6" s="9">
-        <v>23456789</v>
-      </c>
-      <c r="K6" s="3">
+        <v>51906988</v>
+      </c>
+      <c r="K6" s="4">
         <v>6</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="4">
         <v>10</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P6" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+        <v>68</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
-      <c r="A9" s="13"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
-      <c r="A10" s="13"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="12"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1362,24 +1503,92 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="13.550000000000002">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="13.550000000000002">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="13.550000000000002">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="13.550000000000002">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="13.550000000000002">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="13.550000000000002">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="13.550000000000002">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="13.550000000000002">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1391,14 +1600,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -1408,14 +1620,76 @@
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>30</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="13.550000000000002">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="13.550000000000002">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="13.550000000000002">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="13.550000000000002">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="13.550000000000002">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="13.550000000000002">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="13.550000000000002">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="13.550000000000002">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1427,14 +1701,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="8.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -1444,62 +1721,100 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>40</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>40</v>
       </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>30</v>
       </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>30</v>
       </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>30</v>
       </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>30</v>
       </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>30</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="13.550000000000002">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="13.550000000000002">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>